<commit_message>
Sync files with oneDrive
</commit_message>
<xml_diff>
--- a/Docs/AF5/Cronograma Proyecto IMTC.xlsx
+++ b/Docs/AF5/Cronograma Proyecto IMTC.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28619"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="664" documentId="13_ncr:1_{6123CA65-C768-44C9-800C-29ABA8D0CBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{738489FA-D328-4C59-9818-F109CA933C0A}"/>
+  <xr:revisionPtr revIDLastSave="666" documentId="13_ncr:1_{6123CA65-C768-44C9-800C-29ABA8D0CBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F5B9125-B1DF-487B-B14E-07A9DFC20E6C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,11 +14,11 @@
   <definedNames>
     <definedName name="hoy" localSheetId="0">TODAY()</definedName>
     <definedName name="Inicio_del_proyecto">Cronograma!$E$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Cronograma!$4:$6</definedName>
     <definedName name="Semana_para_mostrar">Cronograma!$E$4</definedName>
     <definedName name="task_end" localSheetId="0">Cronograma!$F1</definedName>
     <definedName name="task_progress" localSheetId="0">Cronograma!$D1</definedName>
     <definedName name="task_start" localSheetId="0">Cronograma!$E1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Cronograma!$4:$6</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -359,7 +359,7 @@
     <numFmt numFmtId="169" formatCode="d\ &quot;de&quot;\ mmmm\ &quot;de&quot;\ yyyy"/>
     <numFmt numFmtId="170" formatCode="dd\-mm\-yyyy;@"/>
   </numFmts>
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="39">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1430,12 +1430,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1448,64 +1442,70 @@
     <xf numFmtId="169" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="3" xfId="9">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="3" xfId="9" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
-    <cellStyle name="20% - Accent1" xfId="31" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="43" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="47" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="51" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="32" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="36" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="40" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="44" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="48" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="52" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="41" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="45" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="49" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="53" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="30" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="42" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="46" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="50" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="19" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="23" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="25" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Comma [0]" xfId="14" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Currency" xfId="15" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Currency [0]" xfId="16" builtinId="7" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="31" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="35" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="39" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="43" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="47" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="51" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="32" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="36" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="40" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="44" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="48" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="52" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="33" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="37" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="41" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="45" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="49" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="53" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="18" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="23" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="25" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="24" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="6" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="17" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="30" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="34" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="38" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="42" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="46" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="50" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="21" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Fecha" xfId="10" xr:uid="{229918B6-DD13-4F5A-97B9-305F7E002AA3}"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="18" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="17" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="13" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="19" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Inicio del proyecto" xfId="9" xr:uid="{8EB8A09A-C31C-40A3-B2C1-9449520178B8}"/>
-    <cellStyle name="Input" xfId="21" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="24" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Millares" xfId="4" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Millares [0]" xfId="14" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Moneda" xfId="15" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Moneda [0]" xfId="16" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="20" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Nombre" xfId="11" xr:uid="{B2D3C1EE-6B41-4801-AAFC-C2274E49E503}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Note" xfId="27" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="22" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="27" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="22" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Tarea" xfId="12" xr:uid="{6391D789-272B-4DD2-9BF3-2CDCF610FA41}"/>
-    <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="26" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="5" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="7" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="8" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="29" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="26" builtinId="11" customBuiltin="1"/>
     <cellStyle name="zTextoOculto" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="17">
@@ -1848,10 +1848,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2121,25 +2117,25 @@
   <dimension ref="A1:CG72"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="C1" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="6" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U39" sqref="U39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="43" customWidth="1"/>
-    <col min="2" max="2" width="53.33203125" customWidth="1"/>
-    <col min="3" max="3" width="38.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="3.109375" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" hidden="1" customWidth="1"/>
-    <col min="9" max="15" width="3.33203125" customWidth="1"/>
-    <col min="16" max="85" width="3.109375" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="43" customWidth="1"/>
+    <col min="2" max="2" width="53.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="3.140625" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="15" width="3.28515625" customWidth="1"/>
+    <col min="16" max="85" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:85" ht="30" customHeight="1">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -2151,7 +2147,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="59"/>
     </row>
-    <row r="2" spans="1:85" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:85" ht="30" customHeight="1" thickBot="1">
       <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
@@ -2160,118 +2156,118 @@
       </c>
       <c r="I2" s="60"/>
     </row>
-    <row r="3" spans="1:85" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:85" ht="47.45" customHeight="1">
       <c r="A3" s="43" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="95"/>
+      <c r="D3" s="99"/>
       <c r="E3" s="100">
         <v>45698</v>
       </c>
       <c r="F3" s="100"/>
     </row>
-    <row r="4" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:85" ht="30" customHeight="1">
       <c r="A4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="95"/>
+      <c r="D4" s="99"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="96" t="s">
+      <c r="I4" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
-      <c r="M4" s="97"/>
-      <c r="N4" s="97"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="97"/>
-      <c r="Q4" s="97"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="97"/>
-      <c r="T4" s="97"/>
-      <c r="U4" s="98" t="s">
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="95"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="95"/>
+      <c r="R4" s="95"/>
+      <c r="S4" s="95"/>
+      <c r="T4" s="95"/>
+      <c r="U4" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="V4" s="98"/>
-      <c r="W4" s="98"/>
-      <c r="X4" s="98"/>
-      <c r="Y4" s="98"/>
-      <c r="Z4" s="98"/>
-      <c r="AA4" s="98"/>
-      <c r="AB4" s="98"/>
-      <c r="AC4" s="98"/>
-      <c r="AD4" s="98"/>
-      <c r="AE4" s="98"/>
-      <c r="AF4" s="98"/>
-      <c r="AG4" s="98"/>
-      <c r="AH4" s="98"/>
-      <c r="AI4" s="98"/>
-      <c r="AJ4" s="98"/>
-      <c r="AK4" s="98"/>
-      <c r="AL4" s="98"/>
-      <c r="AM4" s="98"/>
-      <c r="AN4" s="98"/>
-      <c r="AO4" s="98"/>
-      <c r="AP4" s="98"/>
-      <c r="AQ4" s="98"/>
-      <c r="AR4" s="98"/>
-      <c r="AS4" s="98"/>
-      <c r="AT4" s="98"/>
-      <c r="AU4" s="98"/>
-      <c r="AV4" s="98"/>
-      <c r="AW4" s="98"/>
-      <c r="AX4" s="98"/>
-      <c r="AY4" s="98"/>
-      <c r="AZ4" s="99" t="s">
+      <c r="V4" s="96"/>
+      <c r="W4" s="96"/>
+      <c r="X4" s="96"/>
+      <c r="Y4" s="96"/>
+      <c r="Z4" s="96"/>
+      <c r="AA4" s="96"/>
+      <c r="AB4" s="96"/>
+      <c r="AC4" s="96"/>
+      <c r="AD4" s="96"/>
+      <c r="AE4" s="96"/>
+      <c r="AF4" s="96"/>
+      <c r="AG4" s="96"/>
+      <c r="AH4" s="96"/>
+      <c r="AI4" s="96"/>
+      <c r="AJ4" s="96"/>
+      <c r="AK4" s="96"/>
+      <c r="AL4" s="96"/>
+      <c r="AM4" s="96"/>
+      <c r="AN4" s="96"/>
+      <c r="AO4" s="96"/>
+      <c r="AP4" s="96"/>
+      <c r="AQ4" s="96"/>
+      <c r="AR4" s="96"/>
+      <c r="AS4" s="96"/>
+      <c r="AT4" s="96"/>
+      <c r="AU4" s="96"/>
+      <c r="AV4" s="96"/>
+      <c r="AW4" s="96"/>
+      <c r="AX4" s="96"/>
+      <c r="AY4" s="96"/>
+      <c r="AZ4" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="BA4" s="99"/>
-      <c r="BB4" s="99"/>
-      <c r="BC4" s="99"/>
-      <c r="BD4" s="99"/>
-      <c r="BE4" s="99"/>
-      <c r="BF4" s="99"/>
-      <c r="BG4" s="99"/>
-      <c r="BH4" s="99"/>
-      <c r="BI4" s="99"/>
-      <c r="BJ4" s="99"/>
-      <c r="BK4" s="99"/>
-      <c r="BL4" s="99"/>
-      <c r="BM4" s="99"/>
-      <c r="BN4" s="99"/>
-      <c r="BO4" s="99"/>
-      <c r="BP4" s="99"/>
-      <c r="BQ4" s="99"/>
-      <c r="BR4" s="99"/>
-      <c r="BS4" s="99"/>
-      <c r="BT4" s="99"/>
-      <c r="BU4" s="99"/>
-      <c r="BV4" s="99"/>
-      <c r="BW4" s="99"/>
-      <c r="BX4" s="99"/>
-      <c r="BY4" s="99"/>
-      <c r="BZ4" s="99"/>
-      <c r="CA4" s="99"/>
-      <c r="CB4" s="99"/>
-      <c r="CC4" s="99"/>
+      <c r="BA4" s="97"/>
+      <c r="BB4" s="97"/>
+      <c r="BC4" s="97"/>
+      <c r="BD4" s="97"/>
+      <c r="BE4" s="97"/>
+      <c r="BF4" s="97"/>
+      <c r="BG4" s="97"/>
+      <c r="BH4" s="97"/>
+      <c r="BI4" s="97"/>
+      <c r="BJ4" s="97"/>
+      <c r="BK4" s="97"/>
+      <c r="BL4" s="97"/>
+      <c r="BM4" s="97"/>
+      <c r="BN4" s="97"/>
+      <c r="BO4" s="97"/>
+      <c r="BP4" s="97"/>
+      <c r="BQ4" s="97"/>
+      <c r="BR4" s="97"/>
+      <c r="BS4" s="97"/>
+      <c r="BT4" s="97"/>
+      <c r="BU4" s="97"/>
+      <c r="BV4" s="97"/>
+      <c r="BW4" s="97"/>
+      <c r="BX4" s="97"/>
+      <c r="BY4" s="97"/>
+      <c r="BZ4" s="97"/>
+      <c r="CA4" s="97"/>
+      <c r="CB4" s="97"/>
+      <c r="CC4" s="97"/>
       <c r="CD4" s="82"/>
       <c r="CE4" s="82"/>
       <c r="CF4" s="82"/>
       <c r="CG4" s="82"/>
     </row>
-    <row r="5" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:85" ht="30" customHeight="1">
       <c r="A5" s="44" t="s">
         <v>11</v>
       </c>
@@ -2590,7 +2586,7 @@
         <v>45774</v>
       </c>
     </row>
-    <row r="6" spans="1:85" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:85" ht="30" customHeight="1" thickBot="1">
       <c r="A6" s="44" t="s">
         <v>12</v>
       </c>
@@ -2922,7 +2918,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:85" ht="30" customHeight="1">
       <c r="B7" s="46" t="s">
         <v>19</v>
       </c>
@@ -3011,7 +3007,7 @@
       <c r="CF7" s="29"/>
       <c r="CG7" s="29"/>
     </row>
-    <row r="8" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A8" s="44" t="s">
         <v>20</v>
       </c>
@@ -3030,7 +3026,7 @@
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14">
-        <f t="shared" ref="H8:H69" si="24">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H69" ca="1" si="24">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>23</v>
       </c>
       <c r="I8" s="29"/>
@@ -3111,7 +3107,7 @@
       <c r="CF8" s="29"/>
       <c r="CG8" s="29"/>
     </row>
-    <row r="9" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="44" t="s">
         <v>23</v>
       </c>
@@ -3132,7 +3128,7 @@
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>7</v>
       </c>
       <c r="I9" s="29"/>
@@ -3213,7 +3209,7 @@
       <c r="CF9" s="29"/>
       <c r="CG9" s="29"/>
     </row>
-    <row r="10" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A10" s="44" t="s">
         <v>25</v>
       </c>
@@ -3234,7 +3230,7 @@
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>6</v>
       </c>
       <c r="I10" s="29"/>
@@ -3315,7 +3311,7 @@
       <c r="CF10" s="29"/>
       <c r="CG10" s="29"/>
     </row>
-    <row r="11" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A11" s="43"/>
       <c r="B11" s="91" t="s">
         <v>27</v>
@@ -3334,7 +3330,7 @@
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>4</v>
       </c>
       <c r="I11" s="29"/>
@@ -3415,7 +3411,7 @@
       <c r="CF11" s="29"/>
       <c r="CG11" s="29"/>
     </row>
-    <row r="12" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A12" s="43"/>
       <c r="B12" s="91" t="s">
         <v>28</v>
@@ -3434,7 +3430,7 @@
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>4</v>
       </c>
       <c r="I12" s="29"/>
@@ -3515,7 +3511,7 @@
       <c r="CF12" s="29"/>
       <c r="CG12" s="29"/>
     </row>
-    <row r="13" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A13" s="43"/>
       <c r="B13" s="55" t="s">
         <v>29</v>
@@ -3532,7 +3528,7 @@
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>3</v>
       </c>
       <c r="I13" s="29"/>
@@ -3613,7 +3609,7 @@
       <c r="CF13" s="29"/>
       <c r="CG13" s="29"/>
     </row>
-    <row r="14" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A14" s="44" t="s">
         <v>30</v>
       </c>
@@ -3632,7 +3628,7 @@
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>23</v>
       </c>
       <c r="I14" s="29"/>
@@ -3713,7 +3709,7 @@
       <c r="CF14" s="29"/>
       <c r="CG14" s="29"/>
     </row>
-    <row r="15" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A15" s="44"/>
       <c r="B15" s="92" t="s">
         <v>24</v>
@@ -3732,7 +3728,7 @@
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>7</v>
       </c>
       <c r="I15" s="29"/>
@@ -3813,7 +3809,7 @@
       <c r="CF15" s="29"/>
       <c r="CG15" s="29"/>
     </row>
-    <row r="16" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A16" s="43"/>
       <c r="B16" s="92" t="s">
         <v>26</v>
@@ -3832,7 +3828,7 @@
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>6</v>
       </c>
       <c r="I16" s="29"/>
@@ -3913,7 +3909,7 @@
       <c r="CF16" s="29"/>
       <c r="CG16" s="29"/>
     </row>
-    <row r="17" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A17" s="43"/>
       <c r="B17" s="92" t="s">
         <v>27</v>
@@ -3932,7 +3928,7 @@
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>4</v>
       </c>
       <c r="I17" s="29"/>
@@ -4013,7 +4009,7 @@
       <c r="CF17" s="29"/>
       <c r="CG17" s="29"/>
     </row>
-    <row r="18" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A18" s="43"/>
       <c r="B18" s="92" t="s">
         <v>28</v>
@@ -4032,7 +4028,7 @@
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>4</v>
       </c>
       <c r="I18" s="29"/>
@@ -4113,7 +4109,7 @@
       <c r="CF18" s="29"/>
       <c r="CG18" s="29"/>
     </row>
-    <row r="19" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A19" s="43"/>
       <c r="B19" s="56" t="s">
         <v>29</v>
@@ -4132,7 +4128,7 @@
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>3</v>
       </c>
       <c r="I19" s="29"/>
@@ -4213,7 +4209,7 @@
       <c r="CF19" s="29"/>
       <c r="CG19" s="29"/>
     </row>
-    <row r="20" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A20" s="43" t="s">
         <v>32</v>
       </c>
@@ -4234,7 +4230,7 @@
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>23</v>
       </c>
       <c r="I20" s="29"/>
@@ -4315,7 +4311,7 @@
       <c r="CF20" s="29"/>
       <c r="CG20" s="29"/>
     </row>
-    <row r="21" spans="1:85" s="3" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:85" s="3" customFormat="1" ht="33.6" customHeight="1" thickBot="1">
       <c r="A21" s="43"/>
       <c r="B21" s="84" t="s">
         <v>35</v>
@@ -4334,7 +4330,7 @@
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>4</v>
       </c>
       <c r="I21" s="29"/>
@@ -4415,7 +4411,7 @@
       <c r="CF21" s="29"/>
       <c r="CG21" s="29"/>
     </row>
-    <row r="22" spans="1:85" s="3" customFormat="1" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:85" s="3" customFormat="1" ht="28.15" customHeight="1" thickBot="1">
       <c r="A22" s="43"/>
       <c r="B22" s="57" t="s">
         <v>36</v>
@@ -4434,7 +4430,7 @@
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>3</v>
       </c>
       <c r="I22" s="29"/>
@@ -4515,7 +4511,7 @@
       <c r="CF22" s="29"/>
       <c r="CG22" s="29"/>
     </row>
-    <row r="23" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A23" s="43"/>
       <c r="B23" s="57" t="s">
         <v>37</v>
@@ -4534,7 +4530,7 @@
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>4</v>
       </c>
       <c r="I23" s="29"/>
@@ -4615,7 +4611,7 @@
       <c r="CF23" s="29"/>
       <c r="CG23" s="29"/>
     </row>
-    <row r="24" spans="1:85" s="3" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:85" s="3" customFormat="1" ht="39" customHeight="1" thickBot="1">
       <c r="A24" s="43"/>
       <c r="B24" s="84" t="s">
         <v>38</v>
@@ -4634,7 +4630,7 @@
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>3</v>
       </c>
       <c r="I24" s="29"/>
@@ -4715,7 +4711,7 @@
       <c r="CF24" s="29"/>
       <c r="CG24" s="29"/>
     </row>
-    <row r="25" spans="1:85" s="3" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:85" s="3" customFormat="1" ht="55.9" customHeight="1" thickBot="1">
       <c r="A25" s="43"/>
       <c r="B25" s="84" t="s">
         <v>39</v>
@@ -4734,7 +4730,7 @@
       </c>
       <c r="G25" s="14"/>
       <c r="H25" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>3</v>
       </c>
       <c r="I25" s="29"/>
@@ -4815,7 +4811,7 @@
       <c r="CF25" s="29"/>
       <c r="CG25" s="29"/>
     </row>
-    <row r="26" spans="1:85" s="3" customFormat="1" ht="50.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:85" s="3" customFormat="1" ht="50.45" customHeight="1" thickBot="1">
       <c r="A26" s="43"/>
       <c r="B26" s="84" t="s">
         <v>40</v>
@@ -4912,7 +4908,7 @@
       <c r="CF26" s="29"/>
       <c r="CG26" s="29"/>
     </row>
-    <row r="27" spans="1:85" s="3" customFormat="1" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:85" s="3" customFormat="1" ht="55.15" customHeight="1" thickBot="1">
       <c r="A27" s="43"/>
       <c r="B27" s="84" t="s">
         <v>41</v>
@@ -5009,7 +5005,7 @@
       <c r="CF27" s="29"/>
       <c r="CG27" s="29"/>
     </row>
-    <row r="28" spans="1:85" s="3" customFormat="1" ht="37.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:85" s="3" customFormat="1" ht="37.9" customHeight="1" thickBot="1">
       <c r="A28" s="43"/>
       <c r="B28" s="84" t="s">
         <v>42</v>
@@ -5106,7 +5102,7 @@
       <c r="CF28" s="29"/>
       <c r="CG28" s="29"/>
     </row>
-    <row r="29" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A29" s="43"/>
       <c r="B29" s="85" t="s">
         <v>43</v>
@@ -5203,7 +5199,7 @@
       <c r="CF29" s="29"/>
       <c r="CG29" s="29"/>
     </row>
-    <row r="30" spans="1:85" s="3" customFormat="1" ht="40.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:85" s="3" customFormat="1" ht="40.9" customHeight="1" thickBot="1">
       <c r="A30" s="43"/>
       <c r="B30" s="84" t="s">
         <v>44</v>
@@ -5300,7 +5296,7 @@
       <c r="CF30" s="29"/>
       <c r="CG30" s="29"/>
     </row>
-    <row r="31" spans="1:85" s="3" customFormat="1" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:85" s="3" customFormat="1" ht="37.15" customHeight="1" thickBot="1">
       <c r="A31" s="43"/>
       <c r="B31" s="84" t="s">
         <v>45</v>
@@ -5397,7 +5393,7 @@
       <c r="CF31" s="29"/>
       <c r="CG31" s="29"/>
     </row>
-    <row r="32" spans="1:85" s="3" customFormat="1" ht="40.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:85" s="3" customFormat="1" ht="40.9" customHeight="1" thickBot="1">
       <c r="A32" s="43"/>
       <c r="B32" s="84" t="s">
         <v>45</v>
@@ -5494,7 +5490,7 @@
       <c r="CF32" s="29"/>
       <c r="CG32" s="29"/>
     </row>
-    <row r="33" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A33" s="43"/>
       <c r="B33" s="57" t="s">
         <v>46</v>
@@ -5591,7 +5587,7 @@
       <c r="CF33" s="29"/>
       <c r="CG33" s="29"/>
     </row>
-    <row r="34" spans="1:85" s="3" customFormat="1" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:85" s="3" customFormat="1" ht="45.6" customHeight="1" thickBot="1">
       <c r="A34" s="43"/>
       <c r="B34" s="84" t="s">
         <v>47</v>
@@ -5688,7 +5684,7 @@
       <c r="CF34" s="29"/>
       <c r="CG34" s="29"/>
     </row>
-    <row r="35" spans="1:85" s="3" customFormat="1" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:85" s="3" customFormat="1" ht="45.6" customHeight="1" thickBot="1">
       <c r="A35" s="43"/>
       <c r="B35" s="84" t="s">
         <v>48</v>
@@ -5785,7 +5781,7 @@
       <c r="CF35" s="29"/>
       <c r="CG35" s="29"/>
     </row>
-    <row r="36" spans="1:85" s="3" customFormat="1" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:85" s="3" customFormat="1" ht="57.6" customHeight="1" thickBot="1">
       <c r="A36" s="43"/>
       <c r="B36" s="79" t="s">
         <v>49</v>
@@ -5882,7 +5878,7 @@
       <c r="CF36" s="29"/>
       <c r="CG36" s="29"/>
     </row>
-    <row r="37" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A37" s="43"/>
       <c r="B37" s="80" t="s">
         <v>51</v>
@@ -5891,7 +5887,7 @@
         <v>50</v>
       </c>
       <c r="D37" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" s="72">
         <v>45706</v>
@@ -5979,7 +5975,7 @@
       <c r="CF37" s="29"/>
       <c r="CG37" s="29"/>
     </row>
-    <row r="38" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A38" s="43"/>
       <c r="B38" s="80" t="s">
         <v>52</v>
@@ -5988,7 +5984,7 @@
         <v>50</v>
       </c>
       <c r="D38" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="72">
         <v>45710</v>
@@ -6076,7 +6072,7 @@
       <c r="CF38" s="29"/>
       <c r="CG38" s="29"/>
     </row>
-    <row r="39" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A39" s="43"/>
       <c r="B39" s="80" t="s">
         <v>53</v>
@@ -6173,7 +6169,7 @@
       <c r="CF39" s="29"/>
       <c r="CG39" s="29"/>
     </row>
-    <row r="40" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A40" s="43"/>
       <c r="B40" s="80" t="s">
         <v>54</v>
@@ -6270,7 +6266,7 @@
       <c r="CF40" s="29"/>
       <c r="CG40" s="29"/>
     </row>
-    <row r="41" spans="1:85" s="3" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:85" s="3" customFormat="1" ht="60" customHeight="1" thickBot="1">
       <c r="A41" s="43"/>
       <c r="B41" s="79" t="s">
         <v>55</v>
@@ -6367,7 +6363,7 @@
       <c r="CF41" s="29"/>
       <c r="CG41" s="29"/>
     </row>
-    <row r="42" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A42" s="43"/>
       <c r="B42" s="80" t="s">
         <v>56</v>
@@ -6464,7 +6460,7 @@
       <c r="CF42" s="29"/>
       <c r="CG42" s="29"/>
     </row>
-    <row r="43" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A43" s="43"/>
       <c r="B43" s="80" t="s">
         <v>57</v>
@@ -6561,7 +6557,7 @@
       <c r="CF43" s="29"/>
       <c r="CG43" s="29"/>
     </row>
-    <row r="44" spans="1:85" s="3" customFormat="1" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:85" s="3" customFormat="1" ht="54" customHeight="1" thickBot="1">
       <c r="A44" s="43"/>
       <c r="B44" s="79" t="s">
         <v>58</v>
@@ -6658,7 +6654,7 @@
       <c r="CF44" s="29"/>
       <c r="CG44" s="29"/>
     </row>
-    <row r="45" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A45" s="43"/>
       <c r="B45" s="80" t="s">
         <v>59</v>
@@ -6755,7 +6751,7 @@
       <c r="CF45" s="29"/>
       <c r="CG45" s="29"/>
     </row>
-    <row r="46" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A46" s="43" t="s">
         <v>32</v>
       </c>
@@ -6776,7 +6772,7 @@
       </c>
       <c r="G46" s="14"/>
       <c r="H46" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>12</v>
       </c>
       <c r="I46" s="29"/>
@@ -6857,7 +6853,7 @@
       <c r="CF46" s="29"/>
       <c r="CG46" s="29"/>
     </row>
-    <row r="47" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A47" s="43"/>
       <c r="B47" s="80" t="s">
         <v>61</v>
@@ -6876,7 +6872,7 @@
       </c>
       <c r="G47" s="14"/>
       <c r="H47" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>12</v>
       </c>
       <c r="I47" s="29"/>
@@ -6957,7 +6953,7 @@
       <c r="CF47" s="29"/>
       <c r="CG47" s="29"/>
     </row>
-    <row r="48" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A48" s="43"/>
       <c r="B48" s="80" t="s">
         <v>62</v>
@@ -6976,7 +6972,7 @@
       </c>
       <c r="G48" s="14"/>
       <c r="H48" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>7</v>
       </c>
       <c r="I48" s="29"/>
@@ -7057,7 +7053,7 @@
       <c r="CF48" s="29"/>
       <c r="CG48" s="29"/>
     </row>
-    <row r="49" spans="1:85" s="3" customFormat="1" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:85" s="3" customFormat="1" ht="49.15" customHeight="1" thickBot="1">
       <c r="A49" s="43"/>
       <c r="B49" s="79" t="s">
         <v>63</v>
@@ -7076,7 +7072,7 @@
       </c>
       <c r="G49" s="14"/>
       <c r="H49" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>28</v>
       </c>
       <c r="I49" s="29"/>
@@ -7157,7 +7153,7 @@
       <c r="CF49" s="29"/>
       <c r="CG49" s="29"/>
     </row>
-    <row r="50" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A50" s="43"/>
       <c r="B50" s="80" t="s">
         <v>59</v>
@@ -7176,7 +7172,7 @@
       </c>
       <c r="G50" s="14"/>
       <c r="H50" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>7</v>
       </c>
       <c r="I50" s="29"/>
@@ -7257,7 +7253,7 @@
       <c r="CF50" s="29"/>
       <c r="CG50" s="29"/>
     </row>
-    <row r="51" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A51" s="43" t="s">
         <v>32</v>
       </c>
@@ -7278,7 +7274,7 @@
       </c>
       <c r="G51" s="14"/>
       <c r="H51" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>7</v>
       </c>
       <c r="I51" s="29"/>
@@ -7359,7 +7355,7 @@
       <c r="CF51" s="29"/>
       <c r="CG51" s="29"/>
     </row>
-    <row r="52" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A52" s="43"/>
       <c r="B52" s="80" t="s">
         <v>61</v>
@@ -7378,7 +7374,7 @@
       </c>
       <c r="G52" s="14"/>
       <c r="H52" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>7</v>
       </c>
       <c r="I52" s="29"/>
@@ -7459,7 +7455,7 @@
       <c r="CF52" s="29"/>
       <c r="CG52" s="29"/>
     </row>
-    <row r="53" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A53" s="43"/>
       <c r="B53" s="80" t="s">
         <v>62</v>
@@ -7478,7 +7474,7 @@
       </c>
       <c r="G53" s="14"/>
       <c r="H53" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>7</v>
       </c>
       <c r="I53" s="29"/>
@@ -7559,7 +7555,7 @@
       <c r="CF53" s="29"/>
       <c r="CG53" s="29"/>
     </row>
-    <row r="54" spans="1:85" s="3" customFormat="1" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:85" s="3" customFormat="1" ht="46.15" customHeight="1" thickBot="1">
       <c r="A54" s="43"/>
       <c r="B54" s="79" t="s">
         <v>64</v>
@@ -7578,7 +7574,7 @@
       </c>
       <c r="G54" s="14"/>
       <c r="H54" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>21</v>
       </c>
       <c r="I54" s="29"/>
@@ -7659,7 +7655,7 @@
       <c r="CF54" s="29"/>
       <c r="CG54" s="29"/>
     </row>
-    <row r="55" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A55" s="43"/>
       <c r="B55" s="80" t="s">
         <v>59</v>
@@ -7678,7 +7674,7 @@
       </c>
       <c r="G55" s="14"/>
       <c r="H55" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>5</v>
       </c>
       <c r="I55" s="29"/>
@@ -7759,7 +7755,7 @@
       <c r="CF55" s="29"/>
       <c r="CG55" s="29"/>
     </row>
-    <row r="56" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A56" s="43" t="s">
         <v>32</v>
       </c>
@@ -7780,7 +7776,7 @@
       </c>
       <c r="G56" s="14"/>
       <c r="H56" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>7</v>
       </c>
       <c r="I56" s="29"/>
@@ -7861,7 +7857,7 @@
       <c r="CF56" s="29"/>
       <c r="CG56" s="29"/>
     </row>
-    <row r="57" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A57" s="43"/>
       <c r="B57" s="80" t="s">
         <v>61</v>
@@ -7880,7 +7876,7 @@
       </c>
       <c r="G57" s="14"/>
       <c r="H57" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>6</v>
       </c>
       <c r="I57" s="29"/>
@@ -7961,7 +7957,7 @@
       <c r="CF57" s="29"/>
       <c r="CG57" s="29"/>
     </row>
-    <row r="58" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A58" s="43"/>
       <c r="B58" s="80" t="s">
         <v>62</v>
@@ -7980,7 +7976,7 @@
       </c>
       <c r="G58" s="14"/>
       <c r="H58" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>3</v>
       </c>
       <c r="I58" s="29"/>
@@ -8061,7 +8057,7 @@
       <c r="CF58" s="29"/>
       <c r="CG58" s="29"/>
     </row>
-    <row r="59" spans="1:85" s="3" customFormat="1" ht="48.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:85" s="3" customFormat="1" ht="48.6" customHeight="1" thickBot="1">
       <c r="A59" s="43"/>
       <c r="B59" s="79" t="s">
         <v>65</v>
@@ -8080,7 +8076,7 @@
       </c>
       <c r="G59" s="14"/>
       <c r="H59" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>7</v>
       </c>
       <c r="I59" s="29"/>
@@ -8161,7 +8157,7 @@
       <c r="CF59" s="29"/>
       <c r="CG59" s="29"/>
     </row>
-    <row r="60" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A60" s="43"/>
       <c r="B60" s="80" t="s">
         <v>59</v>
@@ -8180,7 +8176,7 @@
       </c>
       <c r="G60" s="14"/>
       <c r="H60" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>2</v>
       </c>
       <c r="I60" s="29"/>
@@ -8261,7 +8257,7 @@
       <c r="CF60" s="29"/>
       <c r="CG60" s="29"/>
     </row>
-    <row r="61" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A61" s="43" t="s">
         <v>32</v>
       </c>
@@ -8282,7 +8278,7 @@
       </c>
       <c r="G61" s="14"/>
       <c r="H61" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>2</v>
       </c>
       <c r="I61" s="29"/>
@@ -8363,7 +8359,7 @@
       <c r="CF61" s="29"/>
       <c r="CG61" s="29"/>
     </row>
-    <row r="62" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A62" s="43"/>
       <c r="B62" s="80" t="s">
         <v>61</v>
@@ -8382,7 +8378,7 @@
       </c>
       <c r="G62" s="14"/>
       <c r="H62" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>2</v>
       </c>
       <c r="I62" s="29"/>
@@ -8463,7 +8459,7 @@
       <c r="CF62" s="29"/>
       <c r="CG62" s="29"/>
     </row>
-    <row r="63" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A63" s="43"/>
       <c r="B63" s="80" t="s">
         <v>62</v>
@@ -8482,7 +8478,7 @@
       </c>
       <c r="G63" s="14"/>
       <c r="H63" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>1</v>
       </c>
       <c r="I63" s="29"/>
@@ -8563,7 +8559,7 @@
       <c r="CF63" s="29"/>
       <c r="CG63" s="29"/>
     </row>
-    <row r="64" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A64" s="43"/>
       <c r="B64" s="79" t="s">
         <v>66</v>
@@ -8582,7 +8578,7 @@
       </c>
       <c r="G64" s="14"/>
       <c r="H64" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>7</v>
       </c>
       <c r="I64" s="29"/>
@@ -8663,7 +8659,7 @@
       <c r="CF64" s="29"/>
       <c r="CG64" s="29"/>
     </row>
-    <row r="65" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A65" s="43"/>
       <c r="B65" s="79" t="s">
         <v>68</v>
@@ -8682,7 +8678,7 @@
       </c>
       <c r="G65" s="14"/>
       <c r="H65" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v>7</v>
       </c>
       <c r="I65" s="29"/>
@@ -8763,13 +8759,13 @@
       <c r="CF65" s="29"/>
       <c r="CG65" s="29"/>
     </row>
-    <row r="66" spans="1:85" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:85" s="3" customFormat="1" ht="15" thickBot="1">
       <c r="A66" s="43" t="s">
         <v>32</v>
       </c>
       <c r="G66" s="14"/>
       <c r="H66" s="14" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="I66" s="29"/>
@@ -8850,13 +8846,13 @@
       <c r="CF66" s="29"/>
       <c r="CG66" s="29"/>
     </row>
-    <row r="67" spans="1:85" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:85" s="3" customFormat="1" ht="15" thickBot="1">
       <c r="A67" s="43" t="s">
         <v>32</v>
       </c>
       <c r="G67" s="14"/>
       <c r="H67" s="14" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="I67" s="29"/>
@@ -8937,7 +8933,7 @@
       <c r="CF67" s="29"/>
       <c r="CG67" s="29"/>
     </row>
-    <row r="68" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A68" s="43" t="s">
         <v>69</v>
       </c>
@@ -8948,7 +8944,7 @@
       <c r="F68" s="73"/>
       <c r="G68" s="14"/>
       <c r="H68" s="14" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="I68" s="29"/>
@@ -9029,7 +9025,7 @@
       <c r="CF68" s="29"/>
       <c r="CG68" s="29"/>
     </row>
-    <row r="69" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A69" s="44" t="s">
         <v>70</v>
       </c>
@@ -9042,7 +9038,7 @@
       <c r="F69" s="75"/>
       <c r="G69" s="28"/>
       <c r="H69" s="28" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="I69" s="31"/>
@@ -9123,14 +9119,14 @@
       <c r="CF69" s="31"/>
       <c r="CG69" s="31"/>
     </row>
-    <row r="70" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:85" ht="30" customHeight="1">
       <c r="G70" s="6"/>
     </row>
-    <row r="71" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:85" ht="30" customHeight="1">
       <c r="C71" s="11"/>
       <c r="F71" s="45"/>
     </row>
-    <row r="72" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:85" ht="30" customHeight="1">
       <c r="C72" s="12"/>
     </row>
   </sheetData>
@@ -9239,86 +9235,86 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.9"/>
   <cols>
-    <col min="1" max="1" width="87.109375" style="33" customWidth="1"/>
-    <col min="2" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="87.140625" style="33" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:2" s="35" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1"/>
+    <row r="2" spans="1:2" s="35" customFormat="1" ht="15.6">
       <c r="A2" s="34" t="s">
         <v>72</v>
       </c>
       <c r="B2" s="34"/>
     </row>
-    <row r="3" spans="1:2" s="39" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="39" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="61" t="s">
         <v>73</v>
       </c>
       <c r="B3" s="40"/>
     </row>
-    <row r="4" spans="1:2" s="36" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" s="36" customFormat="1" ht="25.9">
       <c r="A4" s="37" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1">
       <c r="A5" s="38" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1">
       <c r="A6" s="37" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="33" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" s="33" customFormat="1" ht="228" customHeight="1">
       <c r="A7" s="42" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="36" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2" s="36" customFormat="1" ht="25.9">
       <c r="A8" s="37" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="57.6">
       <c r="A9" s="38" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="33" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" s="33" customFormat="1" ht="27.95" customHeight="1">
       <c r="A10" s="41" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="36" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:2" s="36" customFormat="1" ht="25.9">
       <c r="A11" s="37" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="28.9">
       <c r="A12" s="38" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="33" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" s="33" customFormat="1" ht="27.95" customHeight="1">
       <c r="A13" s="41" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="36" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:2" s="36" customFormat="1" ht="25.9">
       <c r="A14" s="37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="93.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="93.75" customHeight="1">
       <c r="A15" s="38" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="86.45">
       <c r="A16" s="38" t="s">
         <v>86</v>
       </c>
@@ -9337,12 +9333,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9634,69 +9641,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{708DBB9E-6D89-4A94-9DC5-964B7833E11C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{708DBB9E-6D89-4A94-9DC5-964B7833E11C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}"/>
 </file>
</xml_diff>